<commit_message>
Changed , to upper bar in font. And fixed up verillog for simulator that generates the font rom init txt file
</commit_message>
<xml_diff>
--- a/font_5x7_gen.xlsx
+++ b/font_5x7_gen.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecp\fpga_rocket_launcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intelFPGA_lite\fpga_blaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB754F18-0B62-423D-BAB3-EAD1AF996A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C065B9B3-2DB0-4FE5-BEDE-13C999DECE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3128" yWindow="1545" windowWidth="21600" windowHeight="11332" xr2:uid="{3921083B-5F76-4E99-944D-72BF171E8BE5}"/>
+    <workbookView xWindow="-28898" yWindow="-3908" windowWidth="28996" windowHeight="15795" xr2:uid="{3921083B-5F76-4E99-944D-72BF171E8BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -797,9 +798,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -837,7 +838,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -943,7 +944,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1085,7 +1086,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1095,27 +1096,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC6C0D8-6DE1-4EE2-BFB8-90ABFF76D11F}">
   <dimension ref="A1:BJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.59765625" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" customWidth="1"/>
-    <col min="3" max="7" width="2.73046875" customWidth="1"/>
-    <col min="9" max="13" width="2.73046875" customWidth="1"/>
-    <col min="15" max="19" width="2.73046875" customWidth="1"/>
-    <col min="21" max="25" width="2.73046875" customWidth="1"/>
-    <col min="27" max="31" width="2.73046875" customWidth="1"/>
-    <col min="33" max="37" width="2.73046875" customWidth="1"/>
-    <col min="39" max="43" width="2.73046875" customWidth="1"/>
-    <col min="45" max="49" width="2.73046875" customWidth="1"/>
-    <col min="51" max="55" width="2.73046875" customWidth="1"/>
-    <col min="57" max="61" width="2.73046875" customWidth="1"/>
+    <col min="1" max="1" width="76.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="7" width="2.7109375" customWidth="1"/>
+    <col min="9" max="13" width="2.7109375" customWidth="1"/>
+    <col min="15" max="19" width="2.7109375" customWidth="1"/>
+    <col min="21" max="25" width="2.7109375" customWidth="1"/>
+    <col min="27" max="31" width="2.7109375" customWidth="1"/>
+    <col min="33" max="37" width="2.7109375" customWidth="1"/>
+    <col min="39" max="43" width="2.7109375" customWidth="1"/>
+    <col min="45" max="49" width="2.7109375" customWidth="1"/>
+    <col min="51" max="55" width="2.7109375" customWidth="1"/>
+    <col min="57" max="61" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT(H1,N1,T1,Z1,AF1,AL1,AR1,AX1,BD1,BJ1)</f>
         <v>8'h41,8'h42,8'h43,8'h44,8'h45,8'h46,8'h47,8'h48,8'h49,8'h4A,</v>
@@ -1191,7 +1192,7 @@
         <v>8'h4A,</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A32" si="0">_xlfn.CONCAT(H2,N2,T2,Z2,AF2,AL2,AR2,AX2,BD2,BJ2)</f>
         <v>01110_11110_01110_11110_11111_11111_01110_10001_01110_00001_</v>
@@ -1353,7 +1354,7 @@
         <v>00001_</v>
       </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>10001_10001_10001_10001_10000_10000_10001_10001_00100_00001_</v>
@@ -1453,7 +1454,7 @@
         <v>00001_</v>
       </c>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>10001_10001_10000_10001_10000_10000_10000_10001_00100_00001_</v>
@@ -1548,7 +1549,7 @@
         <v>00001_</v>
       </c>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>10001_11110_10000_10001_11110_11110_10111_11111_00100_00001_</v>
@@ -1685,7 +1686,7 @@
         <v>00001_</v>
       </c>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>11111_10001_10000_10001_10000_10000_10001_10001_00100_10001_</v>
@@ -1793,7 +1794,7 @@
         <v>10001_</v>
       </c>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>10001_10001_10001_10001_10000_10000_10001_10001_00100_10001_</v>
@@ -1894,7 +1895,7 @@
         <v>10001_</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>10001_11110_01110_11110_11111_10000_01110_10001_01110_01110_</v>
@@ -2050,7 +2051,7 @@
         <v>01110_</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>8'h4B,8'h4C,8'h4D,8'h4E,8'h4F,8'h50,8'h51,8'h52,8'h53,8'h54,</v>
@@ -2126,7 +2127,7 @@
         <v>8'h54,</v>
       </c>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>10001_10000_10001_10001_01110_11110_01110_11110_01110_11111_</v>
@@ -2280,7 +2281,7 @@
         <v>11111_</v>
       </c>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>10010_10000_11011_11001_10001_10001_10001_10001_10001_00100_</v>
@@ -2393,7 +2394,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>10100_10000_10101_10101_10001_10001_10001_10001_10000_00100_</v>
@@ -2501,7 +2502,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>11000_10000_10101_10011_10001_11110_10001_11110_01110_00100_</v>
@@ -2630,7 +2631,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>10100_10000_10001_10001_10001_10000_10101_10100_00001_00100_</v>
@@ -2734,7 +2735,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>10010_10000_10001_10001_10001_10000_10010_10010_10001_00100_</v>
@@ -2838,7 +2839,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>10001_11111_10001_10001_01110_10000_01101_10001_01110_00100_</v>
@@ -2982,7 +2983,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="17" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>8'h55,8'h56,8'h57,8'h58,8'h59,8'h5A,8'h2E,8'h3A,8'h2F,8'h2C,</v>
@@ -3058,10 +3059,10 @@
         <v>8'h2C,</v>
       </c>
     </row>
-    <row r="18" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>10001_10001_10001_10001_10001_11111_00000_00000_00000_00000_</v>
+        <v>10001_10001_10001_10001_10001_11111_00000_00000_00000_11111_</v>
       </c>
       <c r="C18" s="15">
         <v>1</v>
@@ -3174,17 +3175,27 @@
         <f>_xlfn.CONCAT(DEC2BIN(AY18*16+AZ18*8+BA18*4+BB18*2+BC18,5),"_")</f>
         <v>00000_</v>
       </c>
-      <c r="BE18" s="1"/>
-      <c r="BF18" s="2"/>
-      <c r="BG18" s="2"/>
-      <c r="BH18" s="2"/>
-      <c r="BI18" s="3"/>
+      <c r="BE18" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF18" s="2">
+        <v>1</v>
+      </c>
+      <c r="BG18" s="2">
+        <v>1</v>
+      </c>
+      <c r="BH18" s="2">
+        <v>1</v>
+      </c>
+      <c r="BI18" s="3">
+        <v>1</v>
+      </c>
       <c r="BJ18" t="str">
         <f>_xlfn.CONCAT(DEC2BIN(BE18*16+BF18*8+BG18*4+BH18*2+BI18,5),"_")</f>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
     </row>
-    <row r="19" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>10001_10001_10001_10001_10001_00001_00000_00000_00001_00000_</v>
@@ -3274,7 +3285,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="20" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>10001_10001_10001_01010_10001_00010_00000_00100_00010_00000_</v>
@@ -3371,7 +3382,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="21" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>10001_10001_10101_00100_01010_00100_00000_00000_00100_00000_</v>
@@ -3467,10 +3478,10 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="22" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>10001_10001_10101_01010_00100_01000_00000_00100_01000_01100_</v>
+        <v>10001_10001_10101_01010_00100_01000_00000_00100_01000_00000_</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
@@ -3560,22 +3571,16 @@
         <v>01000_</v>
       </c>
       <c r="BE22" s="4"/>
-      <c r="BF22">
-        <v>1</v>
-      </c>
-      <c r="BG22">
-        <v>1</v>
-      </c>
       <c r="BI22" s="5"/>
       <c r="BJ22" t="str">
         <f t="shared" si="29"/>
-        <v>01100_</v>
+        <v>00000_</v>
       </c>
     </row>
-    <row r="23" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>10001_01010_11011_10001_00100_10000_00000_00000_10000_00100_</v>
+        <v>10001_01010_11011_10001_00100_10000_00000_00000_10000_00000_</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -3663,19 +3668,16 @@
         <v>10000_</v>
       </c>
       <c r="BE23" s="4"/>
-      <c r="BG23">
-        <v>1</v>
-      </c>
       <c r="BI23" s="5"/>
       <c r="BJ23" t="str">
         <f t="shared" si="29"/>
-        <v>00100_</v>
+        <v>00000_</v>
       </c>
     </row>
-    <row r="24" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>01110_00100_10001_10001_00100_11111_00100_00000_00000_01000_</v>
+        <v>01110_00100_10001_10001_00100_11111_00100_00000_00000_00000_</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="16">
@@ -3789,18 +3791,16 @@
         <v>00000_</v>
       </c>
       <c r="BE24" s="6"/>
-      <c r="BF24" s="7">
-        <v>1</v>
-      </c>
+      <c r="BF24" s="7"/>
       <c r="BG24" s="7"/>
       <c r="BH24" s="7"/>
       <c r="BI24" s="8"/>
       <c r="BJ24" t="str">
         <f t="shared" si="29"/>
-        <v>01000_</v>
+        <v>00000_</v>
       </c>
     </row>
-    <row r="25" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>8'h30,8'h31,8'h32,8'h33,8'h34,8'h35,8'h36,8'h37,8'h38,8'h39,</v>
@@ -3876,7 +3876,7 @@
         <v>8'h39,</v>
       </c>
     </row>
-    <row r="26" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>01110_00100_01110_11110_10001_11111_01110_11111_01110_01110_</v>
@@ -4036,7 +4036,7 @@
         <v>01110_</v>
       </c>
     </row>
-    <row r="27" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>10001_01100_10001_00001_10001_10000_10001_00001_10001_10001_</v>
@@ -4138,7 +4138,7 @@
         <v>10001_</v>
       </c>
     </row>
-    <row r="28" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>10011_00100_00001_00001_10001_10000_10000_00001_10001_10001_</v>
@@ -4236,7 +4236,7 @@
         <v>10001_</v>
       </c>
     </row>
-    <row r="29" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>10101_00100_00010_01110_11111_11110_11110_00010_01110_01111_</v>
@@ -4382,7 +4382,7 @@
         <v>01111_</v>
       </c>
     </row>
-    <row r="30" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>11001_00100_00100_00001_00001_00001_10001_00100_10001_00001_</v>
@@ -4480,7 +4480,7 @@
         <v>00001_</v>
       </c>
     </row>
-    <row r="31" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>10001_00100_01000_00001_00001_00001_10001_00100_10001_10001_</v>
@@ -4577,7 +4577,7 @@
         <v>10001_</v>
       </c>
     </row>
-    <row r="32" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>01110_01110_11111_11110_00001_11110_01110_00100_01110_01110_</v>
@@ -4733,7 +4733,7 @@
         <v>01110_</v>
       </c>
     </row>
-    <row r="33" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" ref="A33:A40" si="41">_xlfn.CONCAT(H33,N33,T33,Z33,AF33,AL33,AR33,AX33,BD33,BJ33)</f>
         <v>8'h61,8'h62,8'h63,8'h64,8'h65,8'h66,8'h67,8'h68,8'h69,8'h6A,</v>
@@ -4809,7 +4809,7 @@
         <v>8'h6A,</v>
       </c>
     </row>
-    <row r="34" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="41"/>
         <v>00000_10000_00000_00010_00000_00110_00000_10000_00100_00010_</v>
@@ -4919,7 +4919,7 @@
         <v>00010_</v>
       </c>
     </row>
-    <row r="35" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="41"/>
         <v>01100_10000_01100_00010_01100_01001_01110_10000_00000_00000_</v>
@@ -5024,7 +5024,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="36" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="41"/>
         <v>10010_10000_10010_00010_10010_11100_10010_10000_00100_00010_</v>
@@ -5131,7 +5131,7 @@
         <v>00010_</v>
       </c>
     </row>
-    <row r="37" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="41"/>
         <v>00010_11100_10000_01110_11110_01000_11110_11100_00100_00010_</v>
@@ -5258,7 +5258,7 @@
         <v>00010_</v>
       </c>
     </row>
-    <row r="38" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="41"/>
         <v>01110_10010_10000_10010_10000_01000_00010_10010_00100_00010_</v>
@@ -5364,7 +5364,7 @@
         <v>00010_</v>
       </c>
     </row>
-    <row r="39" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="41"/>
         <v>10010_10010_10010_10010_10010_01000_00010_10010_00100_10010_</v>
@@ -5474,7 +5474,7 @@
         <v>10010_</v>
       </c>
     </row>
-    <row r="40" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="41"/>
         <v>01100_11100_01100_01110_01100_01000_11100_10010_00100_01100_</v>
@@ -5612,7 +5612,7 @@
         <v>01100_</v>
       </c>
     </row>
-    <row r="41" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f t="shared" ref="A41:A48" si="52">_xlfn.CONCAT(H41,N41,T41,Z41,AF41,AL41,AR41,AX41,BD41,BJ41)</f>
         <v>8'h6B,8'h6C,8'h6D,8'h6E,8'h6F,8'h70,8'h71,8'h72,8'h73,8'h74,</v>
@@ -5688,7 +5688,7 @@
         <v>8'h74,</v>
       </c>
     </row>
-    <row r="42" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f t="shared" si="52"/>
         <v>10000_01100_00000_00000_00000_00000_00000_00000_00000_01000_</v>
@@ -5792,7 +5792,7 @@
         <v>01000_</v>
       </c>
     </row>
-    <row r="43" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f t="shared" si="52"/>
         <v>10000_00100_11110_11100_01100_11100_01110_10100_01100_01000_</v>
@@ -5919,7 +5919,7 @@
         <v>01000_</v>
       </c>
     </row>
-    <row r="44" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f t="shared" si="52"/>
         <v>10010_00100_10101_10010_10010_10010_10010_11010_10010_11100_</v>
@@ -6041,7 +6041,7 @@
         <v>11100_</v>
       </c>
     </row>
-    <row r="45" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f t="shared" si="52"/>
         <v>10100_00100_10101_10010_10010_11100_10010_10000_01000_01000_</v>
@@ -6153,7 +6153,7 @@
         <v>01000_</v>
       </c>
     </row>
-    <row r="46" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f t="shared" si="52"/>
         <v>11000_00100_10101_10010_10010_10000_01110_10000_00100_01000_</v>
@@ -6263,7 +6263,7 @@
         <v>01000_</v>
       </c>
     </row>
-    <row r="47" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f t="shared" si="52"/>
         <v>10100_00100_10101_10010_01100_10000_00010_10000_10010_01010_</v>
@@ -6373,7 +6373,7 @@
         <v>01010_</v>
       </c>
     </row>
-    <row r="48" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f t="shared" si="52"/>
         <v>10010_01110_00000_00000_00000_00000_00010_00000_01100_01100_</v>
@@ -6489,7 +6489,7 @@
         <v>01100_</v>
       </c>
     </row>
-    <row r="49" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f t="shared" ref="A49:A56" si="63">_xlfn.CONCAT(H49,N49,T49,Z49,AF49,AL49,AR49,AX49,BD49,BJ49)</f>
         <v>8'h75,8'h76,8'h77,8'h78,8'h79,8'h7A,8'h22,8'h21,8'h3F,8'h2B,</v>
@@ -6565,7 +6565,7 @@
         <v>8'h2B,</v>
       </c>
     </row>
-    <row r="50" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f t="shared" si="63"/>
         <v>00000_00000_00000_00000_00000_00000_01010_00100_01110_00000_</v>
@@ -6673,7 +6673,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="51" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f t="shared" si="63"/>
         <v>10010_10001_10001_10010_10010_11110_01010_00100_10001_00100_</v>
@@ -6789,7 +6789,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="52" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f t="shared" si="63"/>
         <v>10010_10001_10001_10010_10010_00010_00000_00100_10001_00100_</v>
@@ -6891,7 +6891,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="53" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f t="shared" si="63"/>
         <v>10010_10001_10101_01100_01110_00100_00000_00100_00010_11111_</v>
@@ -7010,7 +7010,7 @@
         <v>11111_</v>
       </c>
     </row>
-    <row r="54" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f t="shared" si="63"/>
         <v>10010_01010_10101_10010_00010_01000_00000_00100_00100_00100_</v>
@@ -7114,7 +7114,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="55" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f t="shared" si="63"/>
         <v>01110_00100_01110_10010_00010_10000_00000_00000_00000_00100_</v>
@@ -7214,7 +7214,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="56" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f t="shared" si="63"/>
         <v>00000_00000_00000_00000_11100_11110_00000_00100_00100_00000_</v>
@@ -7328,7 +7328,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="57" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f t="shared" ref="A57:A64" si="74">_xlfn.CONCAT(H57,N57,T57,Z57,AF57,AL57,AR57,AX57,BD57,BJ57)</f>
         <v>8'h2D,8'h23,8'h2A,8'h3C,8'h3E,8'h3D,8'h28,8'h29,8'h24,8'h25,</v>
@@ -7404,7 +7404,7 @@
         <v>8'h25,</v>
       </c>
     </row>
-    <row r="58" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f t="shared" si="74"/>
         <v>00000_01010_00000_00010_10000_00000_00100_01000_01110_11000_</v>
@@ -7522,7 +7522,7 @@
         <v>11000_</v>
       </c>
     </row>
-    <row r="59" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f t="shared" si="74"/>
         <v>00000_01010_00100_00100_01000_00000_01000_00100_10001_11001_</v>
@@ -7620,7 +7620,7 @@
         <v>11001_</v>
       </c>
     </row>
-    <row r="60" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" si="74"/>
         <v>00000_11111_10101_01000_00100_11111_01000_00100_10001_00010_</v>
@@ -7738,7 +7738,7 @@
         <v>00010_</v>
       </c>
     </row>
-    <row r="61" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="74"/>
         <v>11111_01010_01110_10000_00010_00000_01000_00100_10001_00100_</v>
@@ -7850,7 +7850,7 @@
         <v>00100_</v>
       </c>
     </row>
-    <row r="62" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="74"/>
         <v>00000_11111_10101_01000_00100_11111_01000_00100_11011_01000_</v>
@@ -7974,7 +7974,7 @@
         <v>01000_</v>
       </c>
     </row>
-    <row r="63" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" si="74"/>
         <v>00000_01010_00100_00100_01000_00000_01000_00100_01010_10011_</v>
@@ -8074,7 +8074,7 @@
         <v>10011_</v>
       </c>
     </row>
-    <row r="64" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f t="shared" si="74"/>
         <v>00000_01010_00000_00010_10000_00000_00100_01000_11011_00011_</v>
@@ -8194,7 +8194,7 @@
         <v>00011_</v>
       </c>
     </row>
-    <row r="66" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" ref="A66:A73" si="85">_xlfn.CONCAT(H66,N66,T66,Z66,AF66,AL66,AR66,AX66,BD66,BJ66)</f>
         <v>8'h30,8'h31,8'h32,8'h33,8'h34,8'h35,8'h36,8'h37,8'h38,8'h39,</v>
@@ -8270,7 +8270,7 @@
         <v>8'h39,</v>
       </c>
     </row>
-    <row r="67" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="85"/>
         <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
@@ -8366,7 +8366,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="68" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="85"/>
         <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
@@ -8432,7 +8432,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="69" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="85"/>
         <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
@@ -8498,7 +8498,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="70" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="85"/>
         <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
@@ -8564,7 +8564,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="71" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="85"/>
         <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
@@ -8630,7 +8630,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="72" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="85"/>
         <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
@@ -8696,7 +8696,7 @@
         <v>00000_</v>
       </c>
     </row>
-    <row r="73" spans="1:62" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="85"/>
         <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>

</xml_diff>

<commit_message>
Added text chars, Updated font file, ran sim, editted overlay. Commit to gen mif file
</commit_message>
<xml_diff>
--- a/font_5x7_gen.xlsx
+++ b/font_5x7_gen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intelFPGA_lite\fpga_blaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C065B9B3-2DB0-4FE5-BEDE-13C999DECE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B577E74B-BE5B-42B2-A21E-31B2C51E8725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-3908" windowWidth="28996" windowHeight="15795" xr2:uid="{3921083B-5F76-4E99-944D-72BF171E8BE5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>A</t>
   </si>
@@ -246,6 +246,9 @@
   <si>
     <t>%</t>
   </si>
+  <si>
+    <t> </t>
+  </si>
 </sst>
 </file>
 
@@ -387,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -415,11 +418,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="53">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1094,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC6C0D8-6DE1-4EE2-BFB8-90ABFF76D11F}">
-  <dimension ref="A1:BJ73"/>
+  <dimension ref="A1:BJ80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A24"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BM72" sqref="BM72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3062,7 +3074,7 @@
     <row r="18" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>10001_10001_10001_10001_10001_11111_00000_00000_00000_11111_</v>
+        <v>10001_10001_10001_10001_10001_11111_00000_00000_00000_00000_</v>
       </c>
       <c r="C18" s="15">
         <v>1</v>
@@ -3175,24 +3187,14 @@
         <f>_xlfn.CONCAT(DEC2BIN(AY18*16+AZ18*8+BA18*4+BB18*2+BC18,5),"_")</f>
         <v>00000_</v>
       </c>
-      <c r="BE18" s="1">
-        <v>1</v>
-      </c>
-      <c r="BF18" s="2">
-        <v>1</v>
-      </c>
-      <c r="BG18" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH18" s="2">
-        <v>1</v>
-      </c>
-      <c r="BI18" s="3">
-        <v>1</v>
-      </c>
+      <c r="BE18" s="1"/>
+      <c r="BF18" s="2"/>
+      <c r="BG18" s="2"/>
+      <c r="BH18" s="2"/>
+      <c r="BI18" s="3"/>
       <c r="BJ18" t="str">
         <f>_xlfn.CONCAT(DEC2BIN(BE18*16+BF18*8+BG18*4+BH18*2+BI18,5),"_")</f>
-        <v>11111_</v>
+        <v>00000_</v>
       </c>
     </row>
     <row r="19" spans="1:62" x14ac:dyDescent="0.25">
@@ -3481,7 +3483,7 @@
     <row r="22" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>10001_10001_10101_01010_00100_01000_00000_00100_01000_00000_</v>
+        <v>10001_10001_10101_01010_00100_01000_00000_00100_01000_01100_</v>
       </c>
       <c r="C22" s="9">
         <v>1</v>
@@ -3571,16 +3573,22 @@
         <v>01000_</v>
       </c>
       <c r="BE22" s="4"/>
+      <c r="BF22">
+        <v>1</v>
+      </c>
+      <c r="BG22">
+        <v>1</v>
+      </c>
       <c r="BI22" s="5"/>
       <c r="BJ22" t="str">
         <f t="shared" si="29"/>
-        <v>00000_</v>
+        <v>01100_</v>
       </c>
     </row>
     <row r="23" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>10001_01010_11011_10001_00100_10000_00000_00000_10000_00000_</v>
+        <v>10001_01010_11011_10001_00100_10000_00000_00000_10000_00100_</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -3668,16 +3676,19 @@
         <v>10000_</v>
       </c>
       <c r="BE23" s="4"/>
+      <c r="BG23">
+        <v>1</v>
+      </c>
       <c r="BI23" s="5"/>
       <c r="BJ23" t="str">
         <f t="shared" si="29"/>
-        <v>00000_</v>
+        <v>00100_</v>
       </c>
     </row>
     <row r="24" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>01110_00100_10001_10001_00100_11111_00100_00000_00000_00000_</v>
+        <v>01110_00100_10001_10001_00100_11111_00100_00000_00000_01000_</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="16">
@@ -3791,13 +3802,15 @@
         <v>00000_</v>
       </c>
       <c r="BE24" s="6"/>
-      <c r="BF24" s="7"/>
+      <c r="BF24" s="7">
+        <v>1</v>
+      </c>
       <c r="BG24" s="7"/>
       <c r="BH24" s="7"/>
       <c r="BI24" s="8"/>
       <c r="BJ24" t="str">
         <f t="shared" si="29"/>
-        <v>00000_</v>
+        <v>01000_</v>
       </c>
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.25">
@@ -8197,83 +8210,123 @@
     <row r="66" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" ref="A66:A73" si="85">_xlfn.CONCAT(H66,N66,T66,Z66,AF66,AL66,AR66,AX66,BD66,BJ66)</f>
-        <v>8'h30,8'h31,8'h32,8'h33,8'h34,8'h35,8'h36,8'h37,8'h38,8'h39,</v>
-      </c>
-      <c r="C66" s="4">
+        <v>8'hC8,8'hC9,8'hCA,8'hCB,8'hCC,8'hCD,8'hCE,8'hCF,8'hD0,8'hD1,</v>
+      </c>
+      <c r="C66" s="4" t="str">
+        <f>CHAR(200+E66)</f>
+        <v>È</v>
+      </c>
+      <c r="E66" s="28">
         <v>0</v>
       </c>
       <c r="H66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(C66)),",")</f>
-        <v>8'h30,</v>
-      </c>
-      <c r="I66" s="4">
+        <v>8'hC8,</v>
+      </c>
+      <c r="I66" s="4" t="str">
+        <f>CHAR(200+K66)</f>
+        <v>É</v>
+      </c>
+      <c r="K66">
         <v>1</v>
       </c>
       <c r="N66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(I66)),",")</f>
-        <v>8'h31,</v>
-      </c>
-      <c r="O66" s="4">
+        <v>8'hC9,</v>
+      </c>
+      <c r="O66" s="4" t="str">
+        <f>CHAR(200+Q66)</f>
+        <v>Ê</v>
+      </c>
+      <c r="Q66" s="27">
         <v>2</v>
       </c>
       <c r="T66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(O66)),",")</f>
-        <v>8'h32,</v>
-      </c>
-      <c r="U66">
+        <v>8'hCA,</v>
+      </c>
+      <c r="U66" s="4" t="str">
+        <f>CHAR(200+W66)</f>
+        <v>Ë</v>
+      </c>
+      <c r="W66">
         <v>3</v>
       </c>
       <c r="Z66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(U66)),",")</f>
-        <v>8'h33,</v>
-      </c>
-      <c r="AA66">
+        <v>8'hCB,</v>
+      </c>
+      <c r="AA66" s="4" t="str">
+        <f>CHAR(200+AC66)</f>
+        <v>Ì</v>
+      </c>
+      <c r="AC66">
         <v>4</v>
       </c>
       <c r="AF66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AA66)),",")</f>
-        <v>8'h34,</v>
-      </c>
-      <c r="AG66">
+        <v>8'hCC,</v>
+      </c>
+      <c r="AG66" s="4" t="str">
+        <f>CHAR(200+AI66)</f>
+        <v>Í</v>
+      </c>
+      <c r="AI66">
         <v>5</v>
       </c>
       <c r="AL66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AG66)),",")</f>
-        <v>8'h35,</v>
-      </c>
-      <c r="AM66">
+        <v>8'hCD,</v>
+      </c>
+      <c r="AM66" s="4" t="str">
+        <f>CHAR(200+AO66)</f>
+        <v>Î</v>
+      </c>
+      <c r="AO66">
         <v>6</v>
       </c>
       <c r="AR66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AM66)),",")</f>
-        <v>8'h36,</v>
-      </c>
-      <c r="AS66">
+        <v>8'hCE,</v>
+      </c>
+      <c r="AS66" s="4" t="str">
+        <f>CHAR(200+AU66)</f>
+        <v>Ï</v>
+      </c>
+      <c r="AU66" s="27">
         <v>7</v>
       </c>
       <c r="AX66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AS66)),",")</f>
-        <v>8'h37,</v>
-      </c>
-      <c r="AY66">
+        <v>8'hCF,</v>
+      </c>
+      <c r="AY66" s="4" t="str">
+        <f>CHAR(200+BA66)</f>
+        <v>Ð</v>
+      </c>
+      <c r="BA66">
         <v>8</v>
       </c>
       <c r="BD66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AY66)),",")</f>
-        <v>8'h38,</v>
-      </c>
-      <c r="BE66">
+        <v>8'hD0,</v>
+      </c>
+      <c r="BE66" s="4" t="str">
+        <f>CHAR(200+BG66)</f>
+        <v>Ñ</v>
+      </c>
+      <c r="BG66">
         <v>9</v>
       </c>
       <c r="BJ66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(BE66)),",")</f>
-        <v>8'h39,</v>
+        <v>8'hD1,</v>
       </c>
     </row>
     <row r="67" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="85"/>
-        <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
+        <v>00000_11111_11111_11111_00000_00000_11111_00100_00000_11111_</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="2"/>
@@ -8284,32 +8337,62 @@
         <f>_xlfn.CONCAT(DEC2BIN(C67*16+D67*8+E67*4+F67*2+G67,5),"_")</f>
         <v>00000_</v>
       </c>
-      <c r="I67" s="1"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="3"/>
+      <c r="I67" s="1">
+        <v>1</v>
+      </c>
+      <c r="J67" s="2">
+        <v>1</v>
+      </c>
+      <c r="K67" s="2">
+        <v>1</v>
+      </c>
+      <c r="L67" s="2">
+        <v>1</v>
+      </c>
+      <c r="M67" s="3">
+        <v>1</v>
+      </c>
       <c r="N67" t="str">
         <f>_xlfn.CONCAT(DEC2BIN(I67*16+J67*8+K67*4+L67*2+M67,5),"_")</f>
-        <v>00000_</v>
-      </c>
-      <c r="O67" s="1"/>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
-      <c r="R67" s="2"/>
-      <c r="S67" s="3"/>
+        <v>11111_</v>
+      </c>
+      <c r="O67" s="1">
+        <v>1</v>
+      </c>
+      <c r="P67" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="2">
+        <v>1</v>
+      </c>
+      <c r="R67" s="2">
+        <v>1</v>
+      </c>
+      <c r="S67" s="3">
+        <v>1</v>
+      </c>
       <c r="T67" t="str">
         <f>_xlfn.CONCAT(DEC2BIN(O67*16+P67*8+Q67*4+R67*2+S67,5),"_")</f>
-        <v>00000_</v>
-      </c>
-      <c r="U67" s="1"/>
-      <c r="V67" s="2"/>
-      <c r="W67" s="2"/>
-      <c r="X67" s="2"/>
-      <c r="Y67" s="3"/>
+        <v>11111_</v>
+      </c>
+      <c r="U67" s="1">
+        <v>1</v>
+      </c>
+      <c r="V67" s="2">
+        <v>1</v>
+      </c>
+      <c r="W67" s="2">
+        <v>1</v>
+      </c>
+      <c r="X67" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y67" s="3">
+        <v>1</v>
+      </c>
       <c r="Z67" t="str">
         <f>_xlfn.CONCAT(DEC2BIN(U67*16+V67*8+W67*4+X67*2+Y67,5),"_")</f>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
       <c r="AA67" s="1"/>
       <c r="AB67" s="2"/>
@@ -8329,23 +8412,35 @@
         <f>_xlfn.CONCAT(DEC2BIN(AG67*16+AH67*8+AI67*4+AJ67*2+AK67,5),"_")</f>
         <v>00000_</v>
       </c>
-      <c r="AM67" s="1"/>
-      <c r="AN67" s="2"/>
-      <c r="AO67" s="2"/>
-      <c r="AP67" s="2"/>
-      <c r="AQ67" s="3"/>
+      <c r="AM67" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN67" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO67" s="2">
+        <v>1</v>
+      </c>
+      <c r="AP67" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ67" s="3">
+        <v>1</v>
+      </c>
       <c r="AR67" t="str">
         <f>_xlfn.CONCAT(DEC2BIN(AM67*16+AN67*8+AO67*4+AP67*2+AQ67,5),"_")</f>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
       <c r="AS67" s="1"/>
       <c r="AT67" s="2"/>
-      <c r="AU67" s="2"/>
+      <c r="AU67" s="2">
+        <v>1</v>
+      </c>
       <c r="AV67" s="2"/>
       <c r="AW67" s="3"/>
       <c r="AX67" t="str">
         <f>_xlfn.CONCAT(DEC2BIN(AS67*16+AT67*8+AU67*4+AV67*2+AW67,5),"_")</f>
-        <v>00000_</v>
+        <v>00100_</v>
       </c>
       <c r="AY67" s="1"/>
       <c r="AZ67" s="2"/>
@@ -8356,26 +8451,44 @@
         <f>_xlfn.CONCAT(DEC2BIN(AY67*16+AZ67*8+BA67*4+BB67*2+BC67,5),"_")</f>
         <v>00000_</v>
       </c>
-      <c r="BE67" s="1"/>
-      <c r="BF67" s="2"/>
-      <c r="BG67" s="2"/>
-      <c r="BH67" s="2"/>
-      <c r="BI67" s="3"/>
+      <c r="BE67" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF67" s="2">
+        <v>1</v>
+      </c>
+      <c r="BG67" s="2">
+        <v>1</v>
+      </c>
+      <c r="BH67" s="2">
+        <v>1</v>
+      </c>
+      <c r="BI67" s="3">
+        <v>1</v>
+      </c>
       <c r="BJ67" t="str">
         <f>_xlfn.CONCAT(DEC2BIN(BE67*16+BF67*8+BG67*4+BH67*2+BI67,5),"_")</f>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
     </row>
     <row r="68" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" si="85"/>
-        <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
+        <v>00111_00000_11110_01111_00000_00000_11111_01110_00100_11111_</v>
       </c>
       <c r="C68" s="4"/>
-      <c r="G68" s="5"/>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68" s="5">
+        <v>1</v>
+      </c>
       <c r="H68" t="str">
         <f t="shared" ref="H68:H73" si="86">_xlfn.CONCAT(DEC2BIN(C68*16+D68*8+E68*4+F68*2+G68,5),"_")</f>
-        <v>00000_</v>
+        <v>00111_</v>
       </c>
       <c r="I68" s="4"/>
       <c r="M68" s="5"/>
@@ -8383,17 +8496,39 @@
         <f t="shared" ref="N68:N73" si="87">_xlfn.CONCAT(DEC2BIN(I68*16+J68*8+K68*4+L68*2+M68,5),"_")</f>
         <v>00000_</v>
       </c>
-      <c r="O68" s="4"/>
+      <c r="O68" s="4">
+        <v>1</v>
+      </c>
+      <c r="P68">
+        <v>1</v>
+      </c>
+      <c r="Q68">
+        <v>1</v>
+      </c>
+      <c r="R68">
+        <v>1</v>
+      </c>
       <c r="S68" s="5"/>
       <c r="T68" t="str">
         <f t="shared" ref="T68:T73" si="88">_xlfn.CONCAT(DEC2BIN(O68*16+P68*8+Q68*4+R68*2+S68,5),"_")</f>
-        <v>00000_</v>
+        <v>11110_</v>
       </c>
       <c r="U68" s="4"/>
-      <c r="Y68" s="5"/>
+      <c r="V68">
+        <v>1</v>
+      </c>
+      <c r="W68">
+        <v>1</v>
+      </c>
+      <c r="X68">
+        <v>1</v>
+      </c>
+      <c r="Y68" s="5">
+        <v>1</v>
+      </c>
       <c r="Z68" t="str">
         <f t="shared" ref="Z68:Z73" si="89">_xlfn.CONCAT(DEC2BIN(U68*16+V68*8+W68*4+X68*2+Y68,5),"_")</f>
-        <v>00000_</v>
+        <v>01111_</v>
       </c>
       <c r="AA68" s="4"/>
       <c r="AE68" s="5"/>
@@ -8404,44 +8539,85 @@
       <c r="AG68" s="4"/>
       <c r="AK68" s="5"/>
       <c r="AL68" t="str">
-        <f t="shared" ref="AL68:AL73" si="91">_xlfn.CONCAT(DEC2BIN(AG68*16+AH68*8+AI68*4+AJ68*2+AK68,5),"_")</f>
+        <f t="shared" ref="AL68:AL74" si="91">_xlfn.CONCAT(DEC2BIN(AG68*16+AH68*8+AI68*4+AJ68*2+AK68,5),"_")</f>
         <v>00000_</v>
       </c>
-      <c r="AM68" s="4"/>
-      <c r="AQ68" s="5"/>
+      <c r="AM68" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN68">
+        <v>1</v>
+      </c>
+      <c r="AO68">
+        <v>1</v>
+      </c>
+      <c r="AP68">
+        <v>1</v>
+      </c>
+      <c r="AQ68" s="5">
+        <v>1</v>
+      </c>
       <c r="AR68" t="str">
         <f t="shared" ref="AR68:AR73" si="92">_xlfn.CONCAT(DEC2BIN(AM68*16+AN68*8+AO68*4+AP68*2+AQ68,5),"_")</f>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
       <c r="AS68" s="4"/>
+      <c r="AT68">
+        <v>1</v>
+      </c>
+      <c r="AU68">
+        <v>1</v>
+      </c>
+      <c r="AV68">
+        <v>1</v>
+      </c>
       <c r="AW68" s="5"/>
       <c r="AX68" t="str">
         <f t="shared" ref="AX68:AX73" si="93">_xlfn.CONCAT(DEC2BIN(AS68*16+AT68*8+AU68*4+AV68*2+AW68,5),"_")</f>
-        <v>00000_</v>
+        <v>01110_</v>
       </c>
       <c r="AY68" s="4"/>
+      <c r="BA68">
+        <v>1</v>
+      </c>
       <c r="BC68" s="5"/>
       <c r="BD68" t="str">
         <f t="shared" ref="BD68:BD73" si="94">_xlfn.CONCAT(DEC2BIN(AY68*16+AZ68*8+BA68*4+BB68*2+BC68,5),"_")</f>
-        <v>00000_</v>
-      </c>
-      <c r="BE68" s="4"/>
-      <c r="BI68" s="5"/>
+        <v>00100_</v>
+      </c>
+      <c r="BE68" s="4">
+        <v>1</v>
+      </c>
+      <c r="BF68">
+        <v>1</v>
+      </c>
+      <c r="BG68">
+        <v>1</v>
+      </c>
+      <c r="BH68" s="27">
+        <v>1</v>
+      </c>
+      <c r="BI68" s="5">
+        <v>1</v>
+      </c>
       <c r="BJ68" t="str">
-        <f t="shared" ref="BJ68:BJ73" si="95">_xlfn.CONCAT(DEC2BIN(BE68*16+BF68*8+BG68*4+BH68*2+BI68,5),"_")</f>
-        <v>00000_</v>
+        <f t="shared" ref="BJ68:BJ74" si="95">_xlfn.CONCAT(DEC2BIN(BE68*16+BF68*8+BG68*4+BH68*2+BI68,5),"_")</f>
+        <v>11111_</v>
       </c>
     </row>
     <row r="69" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" si="85"/>
-        <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
+        <v>00100_00000_11100_00111_10000_00001_01110_11111_01110_11111_</v>
       </c>
       <c r="C69" s="4"/>
+      <c r="E69">
+        <v>1</v>
+      </c>
       <c r="G69" s="5"/>
       <c r="H69" t="str">
         <f t="shared" si="86"/>
-        <v>00000_</v>
+        <v>00100_</v>
       </c>
       <c r="I69" s="4"/>
       <c r="M69" s="5"/>
@@ -8449,65 +8625,132 @@
         <f t="shared" si="87"/>
         <v>00000_</v>
       </c>
-      <c r="O69" s="4"/>
+      <c r="O69" s="4">
+        <v>1</v>
+      </c>
+      <c r="P69">
+        <v>1</v>
+      </c>
+      <c r="Q69">
+        <v>1</v>
+      </c>
       <c r="S69" s="5"/>
       <c r="T69" t="str">
         <f t="shared" si="88"/>
-        <v>00000_</v>
+        <v>11100_</v>
       </c>
       <c r="U69" s="4"/>
-      <c r="Y69" s="5"/>
+      <c r="W69">
+        <v>1</v>
+      </c>
+      <c r="X69">
+        <v>1</v>
+      </c>
+      <c r="Y69" s="5">
+        <v>1</v>
+      </c>
       <c r="Z69" t="str">
         <f t="shared" si="89"/>
-        <v>00000_</v>
-      </c>
-      <c r="AA69" s="4"/>
+        <v>00111_</v>
+      </c>
+      <c r="AA69" s="4">
+        <v>1</v>
+      </c>
       <c r="AE69" s="5"/>
       <c r="AF69" t="str">
         <f t="shared" si="90"/>
-        <v>00000_</v>
+        <v>10000_</v>
       </c>
       <c r="AG69" s="4"/>
-      <c r="AK69" s="5"/>
+      <c r="AK69" s="5">
+        <v>1</v>
+      </c>
       <c r="AL69" t="str">
         <f t="shared" si="91"/>
-        <v>00000_</v>
+        <v>00001_</v>
       </c>
       <c r="AM69" s="4"/>
+      <c r="AN69">
+        <v>1</v>
+      </c>
+      <c r="AO69">
+        <v>1</v>
+      </c>
+      <c r="AP69" s="27">
+        <v>1</v>
+      </c>
       <c r="AQ69" s="5"/>
       <c r="AR69" t="str">
         <f t="shared" si="92"/>
-        <v>00000_</v>
-      </c>
-      <c r="AS69" s="4"/>
-      <c r="AW69" s="5"/>
+        <v>01110_</v>
+      </c>
+      <c r="AS69" s="4">
+        <v>1</v>
+      </c>
+      <c r="AT69">
+        <v>1</v>
+      </c>
+      <c r="AU69">
+        <v>1</v>
+      </c>
+      <c r="AV69">
+        <v>1</v>
+      </c>
+      <c r="AW69" s="5">
+        <v>1</v>
+      </c>
       <c r="AX69" t="str">
         <f t="shared" si="93"/>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
       <c r="AY69" s="4"/>
+      <c r="AZ69" s="27">
+        <v>1</v>
+      </c>
+      <c r="BA69" s="27">
+        <v>1</v>
+      </c>
+      <c r="BB69">
+        <v>1</v>
+      </c>
       <c r="BC69" s="5"/>
       <c r="BD69" t="str">
         <f t="shared" si="94"/>
-        <v>00000_</v>
-      </c>
-      <c r="BE69" s="4"/>
-      <c r="BI69" s="5"/>
+        <v>01110_</v>
+      </c>
+      <c r="BE69" s="4">
+        <v>1</v>
+      </c>
+      <c r="BF69" s="27">
+        <v>1</v>
+      </c>
+      <c r="BG69">
+        <v>1</v>
+      </c>
+      <c r="BH69" s="27">
+        <v>1</v>
+      </c>
+      <c r="BI69" s="5">
+        <v>1</v>
+      </c>
       <c r="BJ69" t="str">
         <f t="shared" si="95"/>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
     </row>
     <row r="70" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" si="85"/>
-        <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
+        <v>00100_00000_11000_00011_11000_00011_01110_00000_11111_11111_</v>
       </c>
       <c r="C70" s="4"/>
+      <c r="E70">
+        <v>1</v>
+      </c>
       <c r="G70" s="5"/>
       <c r="H70" t="str">
         <f t="shared" si="86"/>
-        <v>00000_</v>
+        <v>00100_</v>
       </c>
       <c r="I70" s="4"/>
       <c r="M70" s="5"/>
@@ -8515,35 +8758,64 @@
         <f t="shared" si="87"/>
         <v>00000_</v>
       </c>
-      <c r="O70" s="4"/>
+      <c r="O70" s="4">
+        <v>1</v>
+      </c>
+      <c r="P70">
+        <v>1</v>
+      </c>
       <c r="S70" s="5"/>
       <c r="T70" t="str">
         <f t="shared" si="88"/>
-        <v>00000_</v>
+        <v>11000_</v>
       </c>
       <c r="U70" s="4"/>
-      <c r="Y70" s="5"/>
+      <c r="X70">
+        <v>1</v>
+      </c>
+      <c r="Y70" s="5">
+        <v>1</v>
+      </c>
       <c r="Z70" t="str">
         <f t="shared" si="89"/>
-        <v>00000_</v>
-      </c>
-      <c r="AA70" s="4"/>
+        <v>00011_</v>
+      </c>
+      <c r="AA70" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB70" s="27">
+        <v>1</v>
+      </c>
       <c r="AE70" s="5"/>
       <c r="AF70" t="str">
         <f t="shared" si="90"/>
-        <v>00000_</v>
+        <v>11000_</v>
       </c>
       <c r="AG70" s="4"/>
-      <c r="AK70" s="5"/>
+      <c r="AJ70">
+        <v>1</v>
+      </c>
+      <c r="AK70" s="5">
+        <v>1</v>
+      </c>
       <c r="AL70" t="str">
         <f t="shared" si="91"/>
-        <v>00000_</v>
+        <v>00011_</v>
       </c>
       <c r="AM70" s="4"/>
+      <c r="AN70" s="27">
+        <v>1</v>
+      </c>
+      <c r="AO70" s="27">
+        <v>1</v>
+      </c>
+      <c r="AP70" s="27">
+        <v>1</v>
+      </c>
       <c r="AQ70" s="5"/>
       <c r="AR70" t="str">
         <f t="shared" si="92"/>
-        <v>00000_</v>
+        <v>01110_</v>
       </c>
       <c r="AS70" s="4"/>
       <c r="AW70" s="5"/>
@@ -8551,29 +8823,63 @@
         <f t="shared" si="93"/>
         <v>00000_</v>
       </c>
-      <c r="AY70" s="4"/>
-      <c r="BC70" s="5"/>
+      <c r="AY70" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ70">
+        <v>1</v>
+      </c>
+      <c r="BA70">
+        <v>1</v>
+      </c>
+      <c r="BB70" s="27">
+        <v>1</v>
+      </c>
+      <c r="BC70" s="5">
+        <v>1</v>
+      </c>
       <c r="BD70" t="str">
         <f t="shared" si="94"/>
-        <v>00000_</v>
-      </c>
-      <c r="BE70" s="4"/>
-      <c r="BI70" s="5"/>
+        <v>11111_</v>
+      </c>
+      <c r="BE70" s="4">
+        <v>1</v>
+      </c>
+      <c r="BF70" s="27">
+        <v>1</v>
+      </c>
+      <c r="BG70" s="27">
+        <v>1</v>
+      </c>
+      <c r="BH70" s="27">
+        <v>1</v>
+      </c>
+      <c r="BI70" s="5">
+        <v>1</v>
+      </c>
       <c r="BJ70" t="str">
         <f t="shared" si="95"/>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
     </row>
     <row r="71" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" si="85"/>
-        <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="G71" s="5"/>
+        <v>10101_00000_10000_00001_11100_00111_00100_00000_01110_11111_</v>
+      </c>
+      <c r="C71" s="4">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" s="27"/>
+      <c r="G71" s="5">
+        <v>1</v>
+      </c>
       <c r="H71" t="str">
         <f t="shared" si="86"/>
-        <v>00000_</v>
+        <v>10101_</v>
       </c>
       <c r="I71" s="4"/>
       <c r="M71" s="5"/>
@@ -8581,35 +8887,59 @@
         <f t="shared" si="87"/>
         <v>00000_</v>
       </c>
-      <c r="O71" s="4"/>
+      <c r="O71" s="4">
+        <v>1</v>
+      </c>
       <c r="S71" s="5"/>
       <c r="T71" t="str">
         <f t="shared" si="88"/>
-        <v>00000_</v>
+        <v>10000_</v>
       </c>
       <c r="U71" s="4"/>
-      <c r="Y71" s="5"/>
+      <c r="Y71" s="5">
+        <v>1</v>
+      </c>
       <c r="Z71" t="str">
         <f t="shared" si="89"/>
-        <v>00000_</v>
-      </c>
-      <c r="AA71" s="4"/>
+        <v>00001_</v>
+      </c>
+      <c r="AA71" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB71">
+        <v>1</v>
+      </c>
+      <c r="AC71" s="27">
+        <v>1</v>
+      </c>
       <c r="AE71" s="5"/>
       <c r="AF71" t="str">
         <f t="shared" si="90"/>
-        <v>00000_</v>
+        <v>11100_</v>
       </c>
       <c r="AG71" s="4"/>
-      <c r="AK71" s="5"/>
+      <c r="AI71">
+        <v>1</v>
+      </c>
+      <c r="AJ71">
+        <v>1</v>
+      </c>
+      <c r="AK71" s="5">
+        <v>1</v>
+      </c>
       <c r="AL71" t="str">
         <f t="shared" si="91"/>
-        <v>00000_</v>
+        <v>00111_</v>
       </c>
       <c r="AM71" s="4"/>
+      <c r="AN71" s="27"/>
+      <c r="AO71" s="27">
+        <v>1</v>
+      </c>
       <c r="AQ71" s="5"/>
       <c r="AR71" t="str">
         <f t="shared" si="92"/>
-        <v>00000_</v>
+        <v>00100_</v>
       </c>
       <c r="AS71" s="4"/>
       <c r="AW71" s="5"/>
@@ -8618,28 +8948,59 @@
         <v>00000_</v>
       </c>
       <c r="AY71" s="4"/>
+      <c r="AZ71">
+        <v>1</v>
+      </c>
+      <c r="BA71">
+        <v>1</v>
+      </c>
+      <c r="BB71">
+        <v>1</v>
+      </c>
       <c r="BC71" s="5"/>
       <c r="BD71" t="str">
         <f t="shared" si="94"/>
-        <v>00000_</v>
-      </c>
-      <c r="BE71" s="4"/>
-      <c r="BI71" s="5"/>
+        <v>01110_</v>
+      </c>
+      <c r="BE71" s="4">
+        <v>1</v>
+      </c>
+      <c r="BF71" s="27">
+        <v>1</v>
+      </c>
+      <c r="BG71" s="27">
+        <v>1</v>
+      </c>
+      <c r="BH71" s="27">
+        <v>1</v>
+      </c>
+      <c r="BI71" s="5">
+        <v>1</v>
+      </c>
       <c r="BJ71" t="str">
         <f t="shared" si="95"/>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
     </row>
     <row r="72" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" si="85"/>
-        <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
+        <v>01110_00000_00000_00000_11110_01111_00100_00000_00100_11111_</v>
       </c>
       <c r="C72" s="4"/>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
       <c r="G72" s="5"/>
       <c r="H72" t="str">
         <f t="shared" si="86"/>
-        <v>00000_</v>
+        <v>01110_</v>
       </c>
       <c r="I72" s="4"/>
       <c r="M72" s="5"/>
@@ -8659,23 +9020,49 @@
         <f t="shared" si="89"/>
         <v>00000_</v>
       </c>
-      <c r="AA72" s="4"/>
+      <c r="AA72" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB72">
+        <v>1</v>
+      </c>
+      <c r="AC72">
+        <v>1</v>
+      </c>
+      <c r="AD72">
+        <v>1</v>
+      </c>
       <c r="AE72" s="5"/>
       <c r="AF72" t="str">
         <f t="shared" si="90"/>
-        <v>00000_</v>
+        <v>11110_</v>
       </c>
       <c r="AG72" s="4"/>
-      <c r="AK72" s="5"/>
+      <c r="AH72">
+        <v>1</v>
+      </c>
+      <c r="AI72">
+        <v>1</v>
+      </c>
+      <c r="AJ72">
+        <v>1</v>
+      </c>
+      <c r="AK72" s="5">
+        <v>1</v>
+      </c>
       <c r="AL72" t="str">
         <f t="shared" si="91"/>
-        <v>00000_</v>
+        <v>01111_</v>
       </c>
       <c r="AM72" s="4"/>
+      <c r="AN72" s="27"/>
+      <c r="AO72" s="27">
+        <v>1</v>
+      </c>
       <c r="AQ72" s="5"/>
       <c r="AR72" t="str">
         <f t="shared" si="92"/>
-        <v>00000_</v>
+        <v>00100_</v>
       </c>
       <c r="AS72" s="4"/>
       <c r="AW72" s="5"/>
@@ -8684,31 +9071,49 @@
         <v>00000_</v>
       </c>
       <c r="AY72" s="4"/>
+      <c r="BA72">
+        <v>1</v>
+      </c>
       <c r="BC72" s="5"/>
       <c r="BD72" t="str">
         <f t="shared" si="94"/>
-        <v>00000_</v>
-      </c>
-      <c r="BE72" s="4"/>
-      <c r="BI72" s="5"/>
+        <v>00100_</v>
+      </c>
+      <c r="BE72" s="4">
+        <v>1</v>
+      </c>
+      <c r="BF72" s="27">
+        <v>1</v>
+      </c>
+      <c r="BG72" s="27">
+        <v>1</v>
+      </c>
+      <c r="BH72" s="27">
+        <v>1</v>
+      </c>
+      <c r="BI72" s="5">
+        <v>1</v>
+      </c>
       <c r="BJ72" t="str">
         <f t="shared" si="95"/>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
     </row>
     <row r="73" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" si="85"/>
-        <v>00000_00000_00000_00000_00000_00000_00000_00000_00000_00000_</v>
+        <v>00100_00000_00000_00000_11111_11111_00000_00000_00000_11111_</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
+      <c r="E73" s="7">
+        <v>1</v>
+      </c>
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
       <c r="H73" t="str">
         <f t="shared" si="86"/>
-        <v>00000_</v>
+        <v>00100_</v>
       </c>
       <c r="I73" s="6"/>
       <c r="J73" s="7"/>
@@ -8737,23 +9142,43 @@
         <f t="shared" si="89"/>
         <v>00000_</v>
       </c>
-      <c r="AA73" s="6"/>
-      <c r="AB73" s="7"/>
-      <c r="AC73" s="7"/>
-      <c r="AD73" s="7"/>
-      <c r="AE73" s="8"/>
+      <c r="AA73" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB73" s="7">
+        <v>1</v>
+      </c>
+      <c r="AC73" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD73" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE73" s="8">
+        <v>1</v>
+      </c>
       <c r="AF73" t="str">
         <f t="shared" si="90"/>
-        <v>00000_</v>
-      </c>
-      <c r="AG73" s="6"/>
-      <c r="AH73" s="7"/>
-      <c r="AI73" s="7"/>
-      <c r="AJ73" s="7"/>
-      <c r="AK73" s="8"/>
+        <v>11111_</v>
+      </c>
+      <c r="AG73" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH73" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI73" s="7">
+        <v>1</v>
+      </c>
+      <c r="AJ73" s="7">
+        <v>1</v>
+      </c>
+      <c r="AK73" s="8">
+        <v>1</v>
+      </c>
       <c r="AL73" t="str">
         <f t="shared" si="91"/>
-        <v>00000_</v>
+        <v>11111_</v>
       </c>
       <c r="AM73" s="6"/>
       <c r="AN73" s="7"/>
@@ -8782,274 +9207,294 @@
         <f t="shared" si="94"/>
         <v>00000_</v>
       </c>
-      <c r="BE73" s="6"/>
-      <c r="BF73" s="7"/>
-      <c r="BG73" s="7"/>
-      <c r="BH73" s="7"/>
-      <c r="BI73" s="8"/>
+      <c r="BE73" s="6">
+        <v>1</v>
+      </c>
+      <c r="BF73" s="7">
+        <v>1</v>
+      </c>
+      <c r="BG73" s="7">
+        <v>1</v>
+      </c>
+      <c r="BH73" s="7">
+        <v>1</v>
+      </c>
+      <c r="BI73" s="8">
+        <v>1</v>
+      </c>
       <c r="BJ73" t="str">
         <f t="shared" si="95"/>
-        <v>00000_</v>
+        <v>11111_</v>
+      </c>
+    </row>
+    <row r="80" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="AJ80" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C34:G40">
-    <cfRule type="cellIs" dxfId="51" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="104" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:G48">
-    <cfRule type="cellIs" dxfId="50" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="84" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:G56">
-    <cfRule type="cellIs" dxfId="49" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="64" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:G64">
-    <cfRule type="cellIs" dxfId="48" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="44" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:G73">
-    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34:M40">
-    <cfRule type="cellIs" dxfId="46" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="102" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42:M48">
-    <cfRule type="cellIs" dxfId="45" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="82" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50:M56">
-    <cfRule type="cellIs" dxfId="44" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="62" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:M64">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I67:M73">
-    <cfRule type="cellIs" dxfId="42" priority="21" operator="equal">
+  <conditionalFormatting sqref="I68:M73">
+    <cfRule type="cellIs" dxfId="43" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O34:S40">
-    <cfRule type="cellIs" dxfId="41" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="100" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O42:S48">
-    <cfRule type="cellIs" dxfId="40" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="80" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O50:S56">
-    <cfRule type="cellIs" dxfId="39" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="60" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O58:S64">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+  <conditionalFormatting sqref="O58:S64 Q66">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O67:S73">
-    <cfRule type="cellIs" dxfId="37" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U34:Y40">
-    <cfRule type="cellIs" dxfId="36" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="98" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U42:Y48">
-    <cfRule type="cellIs" dxfId="35" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="78" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U50:Y56">
-    <cfRule type="cellIs" dxfId="34" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="58" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U58:Y64">
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U67:Y73">
-    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA34:AE40">
-    <cfRule type="cellIs" dxfId="31" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="96" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA42:AE48">
-    <cfRule type="cellIs" dxfId="30" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="76" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA50:AE56">
-    <cfRule type="cellIs" dxfId="29" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="56" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA58:AE64">
-    <cfRule type="cellIs" dxfId="28" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA67:AE73">
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG34:AK40">
-    <cfRule type="cellIs" dxfId="26" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="94" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG42:AK48">
-    <cfRule type="cellIs" dxfId="25" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="74" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG50:AK56">
-    <cfRule type="cellIs" dxfId="24" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="54" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG58:AK64">
-    <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG67:AK73">
-    <cfRule type="cellIs" dxfId="22" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM34:AQ40">
-    <cfRule type="cellIs" dxfId="21" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="92" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM42:AQ48">
-    <cfRule type="cellIs" dxfId="20" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="72" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM50:AQ56">
-    <cfRule type="cellIs" dxfId="19" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="52" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM58:AQ64">
-    <cfRule type="cellIs" dxfId="18" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM67:AQ73">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS18:AW24">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS34:AW40">
-    <cfRule type="cellIs" dxfId="15" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="90" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS42:AW48">
-    <cfRule type="cellIs" dxfId="14" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="70" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS50:AW56">
-    <cfRule type="cellIs" dxfId="13" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS58:AW64">
-    <cfRule type="cellIs" dxfId="12" priority="29" operator="equal">
+  <conditionalFormatting sqref="AS58:AW64 AU66">
+    <cfRule type="cellIs" dxfId="15" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS67:AW73">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY34:BC40">
-    <cfRule type="cellIs" dxfId="10" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="88" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY42:BC48">
-    <cfRule type="cellIs" dxfId="9" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="68" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY50:BC56">
-    <cfRule type="cellIs" dxfId="8" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY58:BC64">
-    <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY67:BC73">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE18:BI24">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE34:BI40">
-    <cfRule type="cellIs" dxfId="4" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="86" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE42:BI48">
-    <cfRule type="cellIs" dxfId="3" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="66" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE50:BI56">
-    <cfRule type="cellIs" dxfId="2" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="46" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE58:BI64">
-    <cfRule type="cellIs" dxfId="1" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE67:BI73">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I67:M67">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Moving special chars into 7-bit ASCII space. Unicode handling during rom building is needed.
</commit_message>
<xml_diff>
--- a/font_5x7_gen.xlsx
+++ b/font_5x7_gen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\intelFPGA_lite\fpga_blaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B577E74B-BE5B-42B2-A21E-31B2C51E8725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9981AACA-5BA8-4011-AECC-8C498FFD39A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-3908" windowWidth="28996" windowHeight="15795" xr2:uid="{3921083B-5F76-4E99-944D-72BF171E8BE5}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -390,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -418,20 +417,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="53">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="52">
     <dxf>
       <fill>
         <patternFill>
@@ -1109,7 +1099,7 @@
   <dimension ref="A1:BJ80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BM72" sqref="BM72"/>
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8210,117 +8200,117 @@
     <row r="66" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" ref="A66:A73" si="85">_xlfn.CONCAT(H66,N66,T66,Z66,AF66,AL66,AR66,AX66,BD66,BJ66)</f>
-        <v>8'hC8,8'hC9,8'hCA,8'hCB,8'hCC,8'hCD,8'hCE,8'hCF,8'hD0,8'hD1,</v>
+        <v>8'h10,8'h11,8'h12,8'h13,8'h14,8'h15,8'h16,8'h17,8'h18,8'h19,</v>
       </c>
       <c r="C66" s="4" t="str">
-        <f>CHAR(200+E66)</f>
-        <v>È</v>
-      </c>
-      <c r="E66" s="28">
+        <f>CHAR(16+E66)</f>
+        <v>_x0010_</v>
+      </c>
+      <c r="E66">
         <v>0</v>
       </c>
       <c r="H66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(C66)),",")</f>
-        <v>8'hC8,</v>
+        <v>8'h10,</v>
       </c>
       <c r="I66" s="4" t="str">
-        <f>CHAR(200+K66)</f>
-        <v>É</v>
+        <f>CHAR(16+K66)</f>
+        <v>_x0011_</v>
       </c>
       <c r="K66">
         <v>1</v>
       </c>
       <c r="N66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(I66)),",")</f>
-        <v>8'hC9,</v>
+        <v>8'h11,</v>
       </c>
       <c r="O66" s="4" t="str">
-        <f>CHAR(200+Q66)</f>
-        <v>Ê</v>
-      </c>
-      <c r="Q66" s="27">
+        <f>CHAR(16+Q66)</f>
+        <v>_x0012_</v>
+      </c>
+      <c r="Q66">
         <v>2</v>
       </c>
       <c r="T66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(O66)),",")</f>
-        <v>8'hCA,</v>
+        <v>8'h12,</v>
       </c>
       <c r="U66" s="4" t="str">
-        <f>CHAR(200+W66)</f>
-        <v>Ë</v>
+        <f>CHAR(16+W66)</f>
+        <v>_x0013_</v>
       </c>
       <c r="W66">
         <v>3</v>
       </c>
       <c r="Z66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(U66)),",")</f>
-        <v>8'hCB,</v>
+        <v>8'h13,</v>
       </c>
       <c r="AA66" s="4" t="str">
-        <f>CHAR(200+AC66)</f>
-        <v>Ì</v>
+        <f>CHAR(16+AC66)</f>
+        <v>_x0014_</v>
       </c>
       <c r="AC66">
         <v>4</v>
       </c>
       <c r="AF66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AA66)),",")</f>
-        <v>8'hCC,</v>
+        <v>8'h14,</v>
       </c>
       <c r="AG66" s="4" t="str">
-        <f>CHAR(200+AI66)</f>
-        <v>Í</v>
+        <f>CHAR(16+AI66)</f>
+        <v>_x0015_</v>
       </c>
       <c r="AI66">
         <v>5</v>
       </c>
       <c r="AL66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AG66)),",")</f>
-        <v>8'hCD,</v>
+        <v>8'h15,</v>
       </c>
       <c r="AM66" s="4" t="str">
-        <f>CHAR(200+AO66)</f>
-        <v>Î</v>
+        <f>CHAR(16+AO66)</f>
+        <v>_x0016_</v>
       </c>
       <c r="AO66">
         <v>6</v>
       </c>
       <c r="AR66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AM66)),",")</f>
-        <v>8'hCE,</v>
+        <v>8'h16,</v>
       </c>
       <c r="AS66" s="4" t="str">
-        <f>CHAR(200+AU66)</f>
-        <v>Ï</v>
-      </c>
-      <c r="AU66" s="27">
+        <f>CHAR(16+AU66)</f>
+        <v>_x0017_</v>
+      </c>
+      <c r="AU66">
         <v>7</v>
       </c>
       <c r="AX66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AS66)),",")</f>
-        <v>8'hCF,</v>
+        <v>8'h17,</v>
       </c>
       <c r="AY66" s="4" t="str">
-        <f>CHAR(200+BA66)</f>
-        <v>Ð</v>
+        <f>CHAR(16+BA66)</f>
+        <v>_x0018_</v>
       </c>
       <c r="BA66">
         <v>8</v>
       </c>
       <c r="BD66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(AY66)),",")</f>
-        <v>8'hD0,</v>
+        <v>8'h18,</v>
       </c>
       <c r="BE66" s="4" t="str">
-        <f>CHAR(200+BG66)</f>
-        <v>Ñ</v>
+        <f>CHAR(16+BG66)</f>
+        <v>_x0019_</v>
       </c>
       <c r="BG66">
         <v>9</v>
       </c>
       <c r="BJ66" t="str">
         <f>_xlfn.CONCAT("8'h",DEC2HEX(CODE(BE66)),",")</f>
-        <v>8'hD1,</v>
+        <v>8'h19,</v>
       </c>
     </row>
     <row r="67" spans="1:62" x14ac:dyDescent="0.25">
@@ -8539,7 +8529,7 @@
       <c r="AG68" s="4"/>
       <c r="AK68" s="5"/>
       <c r="AL68" t="str">
-        <f t="shared" ref="AL68:AL74" si="91">_xlfn.CONCAT(DEC2BIN(AG68*16+AH68*8+AI68*4+AJ68*2+AK68,5),"_")</f>
+        <f t="shared" ref="AL68:AL73" si="91">_xlfn.CONCAT(DEC2BIN(AG68*16+AH68*8+AI68*4+AJ68*2+AK68,5),"_")</f>
         <v>00000_</v>
       </c>
       <c r="AM68" s="4">
@@ -8594,14 +8584,14 @@
       <c r="BG68">
         <v>1</v>
       </c>
-      <c r="BH68" s="27">
+      <c r="BH68">
         <v>1</v>
       </c>
       <c r="BI68" s="5">
         <v>1</v>
       </c>
       <c r="BJ68" t="str">
-        <f t="shared" ref="BJ68:BJ74" si="95">_xlfn.CONCAT(DEC2BIN(BE68*16+BF68*8+BG68*4+BH68*2+BI68,5),"_")</f>
+        <f t="shared" ref="BJ68:BJ73" si="95">_xlfn.CONCAT(DEC2BIN(BE68*16+BF68*8+BG68*4+BH68*2+BI68,5),"_")</f>
         <v>11111_</v>
       </c>
     </row>
@@ -8676,7 +8666,7 @@
       <c r="AO69">
         <v>1</v>
       </c>
-      <c r="AP69" s="27">
+      <c r="AP69">
         <v>1</v>
       </c>
       <c r="AQ69" s="5"/>
@@ -8704,10 +8694,10 @@
         <v>11111_</v>
       </c>
       <c r="AY69" s="4"/>
-      <c r="AZ69" s="27">
-        <v>1</v>
-      </c>
-      <c r="BA69" s="27">
+      <c r="AZ69">
+        <v>1</v>
+      </c>
+      <c r="BA69">
         <v>1</v>
       </c>
       <c r="BB69">
@@ -8721,13 +8711,13 @@
       <c r="BE69" s="4">
         <v>1</v>
       </c>
-      <c r="BF69" s="27">
+      <c r="BF69">
         <v>1</v>
       </c>
       <c r="BG69">
         <v>1</v>
       </c>
-      <c r="BH69" s="27">
+      <c r="BH69">
         <v>1</v>
       </c>
       <c r="BI69" s="5">
@@ -8783,7 +8773,7 @@
       <c r="AA70" s="4">
         <v>1</v>
       </c>
-      <c r="AB70" s="27">
+      <c r="AB70">
         <v>1</v>
       </c>
       <c r="AE70" s="5"/>
@@ -8803,13 +8793,13 @@
         <v>00011_</v>
       </c>
       <c r="AM70" s="4"/>
-      <c r="AN70" s="27">
-        <v>1</v>
-      </c>
-      <c r="AO70" s="27">
-        <v>1</v>
-      </c>
-      <c r="AP70" s="27">
+      <c r="AN70">
+        <v>1</v>
+      </c>
+      <c r="AO70">
+        <v>1</v>
+      </c>
+      <c r="AP70">
         <v>1</v>
       </c>
       <c r="AQ70" s="5"/>
@@ -8832,7 +8822,7 @@
       <c r="BA70">
         <v>1</v>
       </c>
-      <c r="BB70" s="27">
+      <c r="BB70">
         <v>1</v>
       </c>
       <c r="BC70" s="5">
@@ -8845,13 +8835,13 @@
       <c r="BE70" s="4">
         <v>1</v>
       </c>
-      <c r="BF70" s="27">
-        <v>1</v>
-      </c>
-      <c r="BG70" s="27">
-        <v>1</v>
-      </c>
-      <c r="BH70" s="27">
+      <c r="BF70">
+        <v>1</v>
+      </c>
+      <c r="BG70">
+        <v>1</v>
+      </c>
+      <c r="BH70">
         <v>1</v>
       </c>
       <c r="BI70" s="5">
@@ -8873,7 +8863,6 @@
       <c r="E71">
         <v>1</v>
       </c>
-      <c r="F71" s="27"/>
       <c r="G71" s="5">
         <v>1</v>
       </c>
@@ -8909,7 +8898,7 @@
       <c r="AB71">
         <v>1</v>
       </c>
-      <c r="AC71" s="27">
+      <c r="AC71">
         <v>1</v>
       </c>
       <c r="AE71" s="5"/>
@@ -8932,8 +8921,7 @@
         <v>00111_</v>
       </c>
       <c r="AM71" s="4"/>
-      <c r="AN71" s="27"/>
-      <c r="AO71" s="27">
+      <c r="AO71">
         <v>1</v>
       </c>
       <c r="AQ71" s="5"/>
@@ -8965,13 +8953,13 @@
       <c r="BE71" s="4">
         <v>1</v>
       </c>
-      <c r="BF71" s="27">
-        <v>1</v>
-      </c>
-      <c r="BG71" s="27">
-        <v>1</v>
-      </c>
-      <c r="BH71" s="27">
+      <c r="BF71">
+        <v>1</v>
+      </c>
+      <c r="BG71">
+        <v>1</v>
+      </c>
+      <c r="BH71">
         <v>1</v>
       </c>
       <c r="BI71" s="5">
@@ -9055,8 +9043,7 @@
         <v>01111_</v>
       </c>
       <c r="AM72" s="4"/>
-      <c r="AN72" s="27"/>
-      <c r="AO72" s="27">
+      <c r="AO72">
         <v>1</v>
       </c>
       <c r="AQ72" s="5"/>
@@ -9082,13 +9069,13 @@
       <c r="BE72" s="4">
         <v>1</v>
       </c>
-      <c r="BF72" s="27">
-        <v>1</v>
-      </c>
-      <c r="BG72" s="27">
-        <v>1</v>
-      </c>
-      <c r="BH72" s="27">
+      <c r="BF72">
+        <v>1</v>
+      </c>
+      <c r="BG72">
+        <v>1</v>
+      </c>
+      <c r="BH72">
         <v>1</v>
       </c>
       <c r="BI72" s="5">
@@ -9234,257 +9221,257 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C34:G40">
-    <cfRule type="cellIs" dxfId="52" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="104" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:G48">
-    <cfRule type="cellIs" dxfId="51" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="84" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:G56">
-    <cfRule type="cellIs" dxfId="50" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="64" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:G64">
-    <cfRule type="cellIs" dxfId="49" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:G73">
-    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34:M40">
-    <cfRule type="cellIs" dxfId="47" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="102" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42:M48">
-    <cfRule type="cellIs" dxfId="46" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="82" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50:M56">
-    <cfRule type="cellIs" dxfId="45" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="62" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:M64">
-    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I68:M73">
-    <cfRule type="cellIs" dxfId="43" priority="22" operator="equal">
+  <conditionalFormatting sqref="I67:M73">
+    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O34:S40">
-    <cfRule type="cellIs" dxfId="42" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="100" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O42:S48">
-    <cfRule type="cellIs" dxfId="41" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="80" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O50:S56">
-    <cfRule type="cellIs" dxfId="40" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="60" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O58:S64 Q66">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O67:S73">
-    <cfRule type="cellIs" dxfId="38" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U34:Y40">
-    <cfRule type="cellIs" dxfId="37" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="98" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U42:Y48">
-    <cfRule type="cellIs" dxfId="36" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="78" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U50:Y56">
-    <cfRule type="cellIs" dxfId="35" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="58" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U58:Y64">
-    <cfRule type="cellIs" dxfId="34" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U67:Y73">
-    <cfRule type="cellIs" dxfId="33" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA34:AE40">
-    <cfRule type="cellIs" dxfId="32" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="96" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA42:AE48">
-    <cfRule type="cellIs" dxfId="31" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="76" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA50:AE56">
-    <cfRule type="cellIs" dxfId="30" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="56" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA58:AE64">
-    <cfRule type="cellIs" dxfId="29" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA67:AE73">
-    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG34:AK40">
-    <cfRule type="cellIs" dxfId="27" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="94" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG42:AK48">
-    <cfRule type="cellIs" dxfId="26" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="74" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG50:AK56">
-    <cfRule type="cellIs" dxfId="25" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="54" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG58:AK64">
-    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG67:AK73">
-    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM34:AQ40">
-    <cfRule type="cellIs" dxfId="23" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="92" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM42:AQ48">
-    <cfRule type="cellIs" dxfId="22" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="72" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM50:AQ56">
-    <cfRule type="cellIs" dxfId="21" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="52" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM58:AQ64">
-    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="32" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM67:AQ73">
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS18:AW24">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS34:AW40">
-    <cfRule type="cellIs" dxfId="18" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="90" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS42:AW48">
-    <cfRule type="cellIs" dxfId="17" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="70" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS50:AW56">
-    <cfRule type="cellIs" dxfId="16" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS58:AW64 AU66">
-    <cfRule type="cellIs" dxfId="15" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS67:AW73">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY34:BC40">
-    <cfRule type="cellIs" dxfId="13" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="88" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY42:BC48">
-    <cfRule type="cellIs" dxfId="12" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="68" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY50:BC56">
-    <cfRule type="cellIs" dxfId="11" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY58:BC64">
-    <cfRule type="cellIs" dxfId="10" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY67:BC73">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE18:BI24">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE34:BI40">
-    <cfRule type="cellIs" dxfId="7" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="86" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE42:BI48">
-    <cfRule type="cellIs" dxfId="6" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="66" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE50:BI56">
-    <cfRule type="cellIs" dxfId="5" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="46" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE58:BI64">
-    <cfRule type="cellIs" dxfId="4" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9493,11 +9480,6 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I67:M67">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>